<commit_message>
Auto stash before revert of "Update to version 3.2.1"
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/elec/bdsbapcf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-oregon\InputData\elec\BDSBaPCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B11859D-DA9A-2645-998A-DEBA3A0778F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23960" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="458" windowWidth="23963" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDSBaPCF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -145,7 +144,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -283,23 +282,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -335,23 +317,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -527,14 +492,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,7 +507,7 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -550,82 +515,82 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -636,28 +601,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.46484375" customWidth="1"/>
+    <col min="2" max="2" width="23.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -665,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -673,7 +638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -681,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -689,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -697,7 +662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -705,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -713,15 +678,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -729,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -737,7 +702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -745,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -754,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -763,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -772,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -781,13 +746,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>34</v>
       </c>
       <c r="B17">
         <f>B9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Auto stash before revert of "Update to version 3.2.1""
This reverts commit de5933eb75b64ce5f1e094d5b49b07c84ded0e03.
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-oregon\InputData\elec\BDSBaPCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/elec/bdsbapcf/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B11859D-DA9A-2645-998A-DEBA3A0778F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="458" windowWidth="23963" windowHeight="11580"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23960" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDSBaPCF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -144,7 +145,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -282,6 +283,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -317,6 +335,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -492,14 +527,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +542,7 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -515,82 +550,82 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -601,28 +636,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.46484375" customWidth="1"/>
-    <col min="2" max="2" width="23.1328125" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -630,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -638,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -646,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -654,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -662,7 +697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -670,7 +705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -678,15 +713,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -694,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -702,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -710,7 +745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -719,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -728,7 +763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -737,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -746,13 +781,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>34</v>
       </c>
       <c r="B17">
         <f>B9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>